<commit_message>
working on new graph
</commit_message>
<xml_diff>
--- a/corona-server-side-asp.net/Excels/Sections/מדדים מרכזיים/ממוצע מאומתים שבועי.xlsx
+++ b/corona-server-side-asp.net/Excels/Sections/מדדים מרכזיים/ממוצע מאומתים שבועי.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>04.05-10.05</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>average</t>
+  </si>
+  <si>
+    <t>dummy point</t>
   </si>
 </sst>
 </file>
@@ -91,13 +94,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +433,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>14</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
override excel injecting function
</commit_message>
<xml_diff>
--- a/corona-server-side-asp.net/Excels/Sections/מדדים מרכזיים/ממוצע מאומתים שבועי.xlsx
+++ b/corona-server-side-asp.net/Excels/Sections/מדדים מרכזיים/ממוצע מאומתים שבועי.xlsx
@@ -19,19 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>04.05-10.05</t>
-  </si>
-  <si>
-    <t>11.05-17.05</t>
-  </si>
-  <si>
-    <t>18.05-24.05</t>
-  </si>
-  <si>
-    <t>שבוע נוכחי</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>key</t>
   </si>
@@ -42,7 +30,13 @@
     <t>average</t>
   </si>
   <si>
-    <t>dummy point</t>
+    <t>01.06-07.06</t>
+  </si>
+  <si>
+    <t>08.06-14.06</t>
+  </si>
+  <si>
+    <t>15.06-21.06</t>
   </si>
 </sst>
 </file>
@@ -386,60 +380,55 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>8</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>